<commit_message>
ACTUALIZACION DEL EXCEL PANTILLA
</commit_message>
<xml_diff>
--- a/vistas/objetivo/plantilla/FormatoCargaObjetivos.xlsx
+++ b/vistas/objetivo/plantilla/FormatoCargaObjetivos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\taeo\vistas\objetivo\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB0B01AD-FE38-4F75-BFB2-1323AFE846B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3054D6FC-50A1-45AE-9693-3A12870FC4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{E8E6381A-42A8-46BC-BC20-8A5FD1356E71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8E6381A-42A8-46BC-BC20-8A5FD1356E71}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,99 +30,51 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t xml:space="preserve">OPERANTES VERBALES VOCALES (se debe registrar únicamente lo que logra en cada sesión) </t>
   </si>
   <si>
-    <t>0.1 </t>
-  </si>
-  <si>
     <t xml:space="preserve">EMPAREJAMIENTO ESTÍMULO-ESTÍMULO (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS) </t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>ECOICAS (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS)</t>
   </si>
   <si>
-    <t>0.3</t>
-  </si>
-  <si>
     <t>MANDOS (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS)</t>
   </si>
   <si>
-    <t>0.4</t>
-  </si>
-  <si>
     <t>TACTOS (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS)</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>AUTOCLÍTICOS (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS)</t>
   </si>
   <si>
-    <t>0.6</t>
-  </si>
-  <si>
     <t>INTRAVERBALES (APOYAR GENERALIZACIÓN A OTROS CONTEXTOS)</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>SEGMENTOS FINOS</t>
   </si>
   <si>
-    <t>1.1</t>
-  </si>
-  <si>
     <t>AMASAR (DEBE INCLUIR EL PULGAR EN EL AMASADO)</t>
   </si>
   <si>
-    <t>1.1.1</t>
-  </si>
-  <si>
     <t>NIVEL INICIAL (ANTEBRAZO A NIVEL DE LA MESA)</t>
   </si>
   <si>
-    <t>1.1.1.1</t>
-  </si>
-  <si>
     <t>Amasar con mano derecha 5 veces</t>
   </si>
   <si>
-    <t>1.1.1.2</t>
-  </si>
-  <si>
     <t>Amasar con mano izquierda 5 veces</t>
   </si>
   <si>
-    <t>1.1.1.3</t>
-  </si>
-  <si>
     <t>Amasar con mano derecha 8 veces</t>
   </si>
   <si>
-    <t>1.1.1.4</t>
-  </si>
-  <si>
     <t>Amasar con mano izquierda 8 veces</t>
   </si>
   <si>
-    <t>1.1.2</t>
-  </si>
-  <si>
     <t>NIVEL INTERMEDIO (FLEXIÓN DE CODO)</t>
   </si>
   <si>
-    <t>1.1.2.1</t>
-  </si>
-  <si>
     <t>Amasar con mano derecha 10 veces</t>
   </si>
   <si>
@@ -130,23 +82,64 @@
   </si>
   <si>
     <t xml:space="preserve">DESCRIPCION </t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>00.01</t>
+  </si>
+  <si>
+    <t>00.02</t>
+  </si>
+  <si>
+    <t>00.03</t>
+  </si>
+  <si>
+    <t>00.04</t>
+  </si>
+  <si>
+    <t>00.05</t>
+  </si>
+  <si>
+    <t>00.06</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>01.01</t>
+  </si>
+  <si>
+    <t>01.01.01</t>
+  </si>
+  <si>
+    <t>01.01.01.01</t>
+  </si>
+  <si>
+    <t>01.01.01.02</t>
+  </si>
+  <si>
+    <t>01.01.01.03</t>
+  </si>
+  <si>
+    <t>01.01.01.04</t>
+  </si>
+  <si>
+    <t>01.01.02</t>
+  </si>
+  <si>
+    <t>01.01.02.01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,8 +172,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -500,149 +495,149 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="239" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>